<commit_message>
Added an Issues Log to track all issues we are having Added an update responsibility and to-do list Updated Change log
</commit_message>
<xml_diff>
--- a/Documentation/EltasRevenge_ChangeLog.xlsx
+++ b/Documentation/EltasRevenge_ChangeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Class_stuff\ISTA 220\TEAM Projects\EltasRevengeFullGame\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C453FE5-16FA-48AF-837D-B2F1A3367C29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E7B1104-DA48-43D7-9357-38A52FCD474B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7365" windowWidth="29040" windowHeight="15840" xr2:uid="{D15F4308-0492-42DF-9A5E-53D82B8F727B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -57,24 +57,62 @@
     <t>easier for gameplay</t>
   </si>
   <si>
-    <t>game becomes open world</t>
-  </si>
-  <si>
     <t>removed maze class, replaced it with ER_Game</t>
   </si>
   <si>
-    <t>Easier to organize</t>
-  </si>
-  <si>
     <t>Namespaces</t>
+  </si>
+  <si>
+    <t>JK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changed Title </t>
+  </si>
+  <si>
+    <t>easier to organize</t>
+  </si>
+  <si>
+    <t>Sounds Better</t>
+  </si>
+  <si>
+    <t>Title page, documentation</t>
+  </si>
+  <si>
+    <t>WP</t>
+  </si>
+  <si>
+    <t>removed audio option</t>
+  </si>
+  <si>
+    <t>unable to use with .netCore</t>
+  </si>
+  <si>
+    <t>player exp</t>
+  </si>
+  <si>
+    <t>Added load screen art</t>
+  </si>
+  <si>
+    <t>allows complete transisitions</t>
+  </si>
+  <si>
+    <t>Game is now open world</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -123,18 +161,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -453,7 +499,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -464,20 +510,20 @@
     <col min="5" max="5" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -485,251 +531,281 @@
       <c r="A2" s="4">
         <v>44044</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>8</v>
+      <c r="E2" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>44044</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="5" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>44044</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>44044</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>44044</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
-      <c r="E33" s="5"/>
+      <c r="E33" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;LChange Log&amp;C&amp;18Elta's Revenge&amp;RTEAM 2</oddHeader>
+    <oddHeader>&amp;LChange Log&amp;C&amp;18Elta's Revenge ChangeLog&amp;RTEAM 2</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>